<commit_message>
updated version of the create_chart method
</commit_message>
<xml_diff>
--- a/custom_excel.xlsx
+++ b/custom_excel.xlsx
@@ -9,7 +9,9 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Payments" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Payments'!$A$1:$C$3</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -17,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -32,8 +34,11 @@
     <font>
       <sz val="11"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -58,6 +63,12 @@
         <bgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00AAAAAA"/>
+        <bgColor rgb="00AAAAAA"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -71,8 +82,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -166,7 +180,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Product Pricing</a:t>
+              <a:t>Sales Data</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -181,7 +195,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Payments'!I2</f>
+              <f>'Payments'!B2</f>
             </strRef>
           </tx>
           <spPr>
@@ -191,7 +205,7 @@
           </spPr>
           <val>
             <numRef>
-              <f>'Payments'!$I$3:$I$10</f>
+              <f>'Payments'!$B$3:$B$10</f>
             </numRef>
           </val>
         </ser>
@@ -200,7 +214,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Payments'!J2</f>
+              <f>'Payments'!C2</f>
             </strRef>
           </tx>
           <spPr>
@@ -210,7 +224,7 @@
           </spPr>
           <val>
             <numRef>
-              <f>'Payments'!$J$3:$J$10</f>
+              <f>'Payments'!$C$3:$C$10</f>
             </numRef>
           </val>
         </ser>
@@ -219,7 +233,7 @@
           <order val="2"/>
           <tx>
             <strRef>
-              <f>'Payments'!K2</f>
+              <f>'Payments'!D2</f>
             </strRef>
           </tx>
           <spPr>
@@ -229,7 +243,7 @@
           </spPr>
           <val>
             <numRef>
-              <f>'Payments'!$K$3:$K$10</f>
+              <f>'Payments'!$D$3:$D$10</f>
             </numRef>
           </val>
         </ser>
@@ -238,7 +252,7 @@
           <order val="3"/>
           <tx>
             <strRef>
-              <f>'Payments'!L2</f>
+              <f>'Payments'!E2</f>
             </strRef>
           </tx>
           <spPr>
@@ -248,10 +262,13 @@
           </spPr>
           <val>
             <numRef>
-              <f>'Payments'!$L$3:$L$10</f>
+              <f>'Payments'!$E$3:$E$10</f>
             </numRef>
           </val>
         </ser>
+        <dLbls>
+          <showVal val="1"/>
+        </dLbls>
         <gapWidth val="150"/>
         <axId val="10"/>
         <axId val="100"/>
@@ -262,6 +279,21 @@
           <orientation val="minMax"/>
         </scaling>
         <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Products</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <crossAx val="100"/>
@@ -274,6 +306,21 @@
         </scaling>
         <axPos val="l"/>
         <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Sales</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <crossAx val="10"/>
@@ -288,13 +335,176 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Price, Tax, and Discount Comparison</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Payments'!I1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Payments'!$I$2:$I$3</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'Payments'!J1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Payments'!$J$2:$J$3</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <strRef>
+              <f>'Payments'!K1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Payments'!$K$2:$K$3</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showVal val="1"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Category</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Amount</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>ExcelCreator</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>This is the name column</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>4</col>
+      <col>7</col>
       <colOff>0</colOff>
-      <row>14</row>
+      <row>9</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -307,6 +517,28 @@
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>22</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -654,278 +886,276 @@
           <t>DATA_PAGAMENTO</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>CRIADO_POR</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>EMPRESA_FACTURACAO</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>PRODUTO</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>ITEM</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>COD_MATERIAL</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>PRECO_BASE</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>IMPOSTO</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
         <is>
           <t>DESCONTO</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" s="2" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" s="2" t="inlineStr">
         <is>
           <t>METODO_PAGAMENTO</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" s="2" t="inlineStr">
         <is>
           <t>ESTADO</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" s="2" t="inlineStr">
         <is>
           <t>ENCOMENDA</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" s="2" t="inlineStr">
         <is>
           <t>PAGAMENTO_AGREGADOR</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" s="2" t="inlineStr">
         <is>
           <t>COD_LOJA_SAP</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="R1" s="2" t="inlineStr">
         <is>
           <t>NOME_LOJA</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="S1" s="2" t="inlineStr">
         <is>
           <t>COD_CLIENTE</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="T1" s="2" t="inlineStr">
         <is>
           <t>NOME_CLIENTE</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="U1" s="2" t="inlineStr">
         <is>
           <t>CLASSE_PAGAMENTO</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <v>12345</v>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>2024-10-10</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="D2" s="3">
+        <f>B2*2</f>
+        <v/>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>Empresa XYZ</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>Produto A</t>
         </is>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="H2" s="3" t="inlineStr">
         <is>
           <t>M123</t>
         </is>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="I2" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="J2" s="2" t="n">
+      <c r="J2" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="K2" s="2" t="n">
+      <c r="K2" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="L2" s="2" t="n">
+      <c r="L2" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="M2" s="2" t="inlineStr">
+      <c r="M2" s="3" t="inlineStr">
         <is>
           <t>Cartao</t>
         </is>
       </c>
-      <c r="N2" s="2" t="inlineStr">
+      <c r="N2" s="3" t="inlineStr">
         <is>
           <t>Pago</t>
         </is>
       </c>
-      <c r="O2" s="2" t="inlineStr">
+      <c r="O2" s="3" t="inlineStr">
         <is>
           <t>ENC001</t>
         </is>
       </c>
-      <c r="P2" s="2" t="inlineStr">
+      <c r="P2" s="3" t="inlineStr">
         <is>
           <t>AGREG001</t>
         </is>
       </c>
-      <c r="Q2" s="2" t="inlineStr">
+      <c r="Q2" s="3" t="inlineStr">
         <is>
           <t>SAP001</t>
         </is>
       </c>
-      <c r="R2" s="2" t="inlineStr">
+      <c r="R2" s="3" t="inlineStr">
         <is>
           <t>Loja Central</t>
         </is>
       </c>
-      <c r="S2" s="2" t="inlineStr">
+      <c r="S2" s="3" t="inlineStr">
         <is>
           <t>C001</t>
         </is>
       </c>
-      <c r="T2" s="2" t="inlineStr">
+      <c r="T2" s="3" t="inlineStr">
         <is>
           <t>Cliente 1</t>
         </is>
       </c>
-      <c r="U2" s="2" t="inlineStr">
+      <c r="U2" s="3" t="inlineStr">
         <is>
           <t>CLASSE_A</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="4" t="n">
         <v>12346</v>
       </c>
-      <c r="C3" s="3" t="inlineStr">
+      <c r="C3" s="4" t="inlineStr">
         <is>
           <t>2024-10-11</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>user1</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="D3" s="4">
+        <f>B2*2</f>
+        <v/>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
         <is>
           <t>Empresa ABC</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="F3" s="4" t="inlineStr">
         <is>
           <t>Produto B</t>
         </is>
       </c>
-      <c r="G3" s="3" t="n">
+      <c r="G3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="H3" s="3" t="inlineStr">
+      <c r="H3" s="4" t="inlineStr">
         <is>
           <t>M124</t>
         </is>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="4" t="n">
         <v>200</v>
       </c>
-      <c r="J3" s="3" t="n">
+      <c r="J3" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="K3" s="3" t="n">
+      <c r="K3" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="L3" s="3" t="n">
+      <c r="L3" s="4" t="n">
         <v>190</v>
       </c>
-      <c r="M3" s="3" t="inlineStr">
+      <c r="M3" s="4" t="inlineStr">
         <is>
           <t>Boleto</t>
         </is>
       </c>
-      <c r="N3" s="3" t="inlineStr">
+      <c r="N3" s="4" t="inlineStr">
         <is>
           <t>Aguardando</t>
         </is>
       </c>
-      <c r="O3" s="3" t="inlineStr">
+      <c r="O3" s="4" t="inlineStr">
         <is>
           <t>ENC002</t>
         </is>
       </c>
-      <c r="P3" s="3" t="inlineStr">
+      <c r="P3" s="4" t="inlineStr">
         <is>
           <t>AGREG002</t>
         </is>
       </c>
-      <c r="Q3" s="3" t="inlineStr">
+      <c r="Q3" s="4" t="inlineStr">
         <is>
           <t>SAP002</t>
         </is>
       </c>
-      <c r="R3" s="3" t="inlineStr">
+      <c r="R3" s="4" t="inlineStr">
         <is>
           <t>Loja Norte</t>
         </is>
       </c>
-      <c r="S3" s="3" t="inlineStr">
+      <c r="S3" s="4" t="inlineStr">
         <is>
           <t>C002</t>
         </is>
       </c>
-      <c r="T3" s="3" t="inlineStr">
+      <c r="T3" s="4" t="inlineStr">
         <is>
           <t>Cliente 2</t>
         </is>
       </c>
-      <c r="U3" s="3" t="inlineStr">
+      <c r="U3" s="4" t="inlineStr">
         <is>
           <t>CLASSE_B</t>
         </is>
@@ -939,6 +1169,7 @@
     <row r="9"/>
     <row r="10"/>
   </sheetData>
+  <autoFilter ref="A1:C3"/>
   <conditionalFormatting sqref="K2:K3">
     <cfRule type="colorScale" priority="1">
       <colorScale>
@@ -955,6 +1186,8 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>